<commit_message>
The complete project has been done with Extent reports,cucumber reports,Scenario report,Automation testing excel file
</commit_message>
<xml_diff>
--- a/target/test-classes/testdata/inputdata.xlsx
+++ b/target/test-classes/testdata/inputdata.xlsx
@@ -605,7 +605,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -665,7 +665,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="4">
-        <v>8438542755</v>
+        <v>8015332963</v>
       </c>
       <c r="D2" s="4">
         <v>12345</v>

</xml_diff>